<commit_message>
advanced hypothesis test workbook
</commit_message>
<xml_diff>
--- a/Test Hypothesis WIth Data/AdvancedTestHypothesis/CaseStudy-Graded/Graded Assignment Dataset- Statistics.xlsx
+++ b/Test Hypothesis WIth Data/AdvancedTestHypothesis/CaseStudy-Graded/Graded Assignment Dataset- Statistics.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\JGA\Content\DSS Redo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Personal\3GitHub\JigsawRepository\Test Hypothesis WIth Data\AdvancedTestHypothesis\CaseStudy-Graded\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -17,7 +17,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$BJ$109</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -95,7 +95,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -408,15 +408,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T109"/>
+  <dimension ref="A1:V109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R82" sqref="R82"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="V6" sqref="V6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -478,7 +478,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -541,7 +541,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>39</v>
       </c>
@@ -604,7 +604,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>40</v>
       </c>
@@ -666,8 +666,11 @@
       <c r="T4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="V4">
+        <v>589.77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>47</v>
       </c>
@@ -729,8 +732,11 @@
       <c r="T5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="V5">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>55</v>
       </c>
@@ -792,8 +798,12 @@
       <c r="T6" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="V6" t="e">
+        <f>CHITEST(D2:D109,V5)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>64</v>
       </c>
@@ -856,7 +866,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>84</v>
       </c>
@@ -919,7 +929,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>106</v>
       </c>
@@ -982,7 +992,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>115</v>
       </c>
@@ -1045,7 +1055,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>129</v>
       </c>
@@ -1108,7 +1118,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>145</v>
       </c>
@@ -1171,7 +1181,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>157</v>
       </c>
@@ -1234,7 +1244,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>159</v>
       </c>
@@ -1297,7 +1307,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>208</v>
       </c>
@@ -1360,7 +1370,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>211</v>
       </c>
@@ -1423,7 +1433,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>214</v>
       </c>
@@ -1486,7 +1496,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>218</v>
       </c>
@@ -1549,7 +1559,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>219</v>
       </c>
@@ -1612,7 +1622,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>220</v>
       </c>
@@ -1675,7 +1685,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>221</v>
       </c>
@@ -1738,7 +1748,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>224</v>
       </c>
@@ -1801,7 +1811,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>232</v>
       </c>
@@ -1864,7 +1874,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>240</v>
       </c>
@@ -1927,7 +1937,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>243</v>
       </c>
@@ -1990,7 +2000,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>247</v>
       </c>
@@ -2053,7 +2063,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>248</v>
       </c>
@@ -2116,7 +2126,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>254</v>
       </c>
@@ -2179,7 +2189,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>256</v>
       </c>
@@ -2242,7 +2252,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>258</v>
       </c>
@@ -2305,7 +2315,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>262</v>
       </c>
@@ -2368,7 +2378,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>263</v>
       </c>
@@ -2431,7 +2441,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>267</v>
       </c>
@@ -2494,7 +2504,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>275</v>
       </c>
@@ -2557,7 +2567,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>276</v>
       </c>
@@ -2620,7 +2630,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>278</v>
       </c>
@@ -2683,7 +2693,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>280</v>
       </c>
@@ -2746,7 +2756,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>291</v>
       </c>
@@ -2809,7 +2819,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>296</v>
       </c>
@@ -2872,7 +2882,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>300</v>
       </c>
@@ -2935,7 +2945,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>301</v>
       </c>
@@ -2998,7 +3008,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>310</v>
       </c>
@@ -3061,7 +3071,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>312</v>
       </c>
@@ -3124,7 +3134,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>319</v>
       </c>
@@ -3187,7 +3197,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>320</v>
       </c>
@@ -3250,7 +3260,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>325</v>
       </c>
@@ -3313,7 +3323,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>337</v>
       </c>
@@ -3376,7 +3386,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>338</v>
       </c>
@@ -3439,7 +3449,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>340</v>
       </c>
@@ -3502,7 +3512,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>341</v>
       </c>
@@ -3565,7 +3575,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>343</v>
       </c>
@@ -3628,7 +3638,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>344</v>
       </c>
@@ -3691,7 +3701,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>345</v>
       </c>
@@ -3754,7 +3764,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>353</v>
       </c>
@@ -3817,7 +3827,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>364</v>
       </c>
@@ -3880,7 +3890,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>365</v>
       </c>
@@ -3943,7 +3953,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>366</v>
       </c>
@@ -4006,7 +4016,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>369</v>
       </c>
@@ -4069,7 +4079,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="59" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>371</v>
       </c>
@@ -4132,7 +4142,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="60" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>374</v>
       </c>
@@ -4195,7 +4205,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="61" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>379</v>
       </c>
@@ -4258,7 +4268,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="62" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>380</v>
       </c>
@@ -4321,7 +4331,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="63" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>384</v>
       </c>
@@ -4384,7 +4394,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="64" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>385</v>
       </c>
@@ -4447,7 +4457,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="65" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>386</v>
       </c>
@@ -4510,7 +4520,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="66" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>389</v>
       </c>
@@ -4573,7 +4583,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="67" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>392</v>
       </c>
@@ -4636,7 +4646,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="68" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>394</v>
       </c>
@@ -4699,7 +4709,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="69" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>406</v>
       </c>
@@ -4762,7 +4772,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="70" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>412</v>
       </c>
@@ -4825,7 +4835,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="71" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>417</v>
       </c>
@@ -4888,7 +4898,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="72" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>421</v>
       </c>
@@ -4951,7 +4961,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="73" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>422</v>
       </c>
@@ -5014,7 +5024,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="74" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>439</v>
       </c>
@@ -5077,7 +5087,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="75" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>450</v>
       </c>
@@ -5140,7 +5150,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="76" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>453</v>
       </c>
@@ -5203,7 +5213,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="77" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>458</v>
       </c>
@@ -5266,7 +5276,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="78" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>464</v>
       </c>
@@ -5329,7 +5339,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="79" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>469</v>
       </c>
@@ -5392,7 +5402,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="80" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>470</v>
       </c>
@@ -5455,7 +5465,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="81" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>473</v>
       </c>
@@ -5518,7 +5528,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="82" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>479</v>
       </c>
@@ -5581,7 +5591,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="83" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>482</v>
       </c>
@@ -5644,7 +5654,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="84" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>484</v>
       </c>
@@ -5707,7 +5717,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="85" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>487</v>
       </c>
@@ -5770,7 +5780,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="86" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>491</v>
       </c>
@@ -5833,7 +5843,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="87" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>493</v>
       </c>
@@ -5896,7 +5906,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="88" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>496</v>
       </c>
@@ -5959,7 +5969,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="89" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>503</v>
       </c>
@@ -6022,7 +6032,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="90" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>506</v>
       </c>
@@ -6085,7 +6095,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="91" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>514</v>
       </c>
@@ -6148,7 +6158,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="92" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>518</v>
       </c>
@@ -6211,7 +6221,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="93" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>519</v>
       </c>
@@ -6274,7 +6284,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="94" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>520</v>
       </c>
@@ -6337,7 +6347,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="95" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>521</v>
       </c>
@@ -6400,7 +6410,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="96" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>523</v>
       </c>
@@ -6463,7 +6473,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="97" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>524</v>
       </c>
@@ -6526,7 +6536,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="98" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>526</v>
       </c>
@@ -6589,7 +6599,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="99" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>528</v>
       </c>
@@ -6652,7 +6662,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="100" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>535</v>
       </c>
@@ -6715,7 +6725,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="101" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>536</v>
       </c>
@@ -6778,7 +6788,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="102" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>538</v>
       </c>
@@ -6841,7 +6851,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="103" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>540</v>
       </c>
@@ -6904,7 +6914,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="104" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>543</v>
       </c>
@@ -6967,7 +6977,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="105" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>552</v>
       </c>
@@ -7030,7 +7040,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="106" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>555</v>
       </c>
@@ -7093,7 +7103,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="107" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>557</v>
       </c>
@@ -7156,7 +7166,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="108" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>560</v>
       </c>
@@ -7218,8 +7228,11 @@
       <c r="T108" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="109" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="V108">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="109" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>561</v>
       </c>

</xml_diff>